<commit_message>
Modificacion sobre acciones correctivas Febrero
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-150227.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-150227.xlsx
@@ -179,16 +179,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda 2" xfId="2"/>
@@ -512,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -533,30 +535,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C4" s="9" t="s">
@@ -585,10 +587,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -620,7 +622,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -630,7 +632,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -640,7 +642,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -650,7 +652,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -660,7 +662,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -670,7 +672,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -680,7 +682,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -690,7 +692,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -700,7 +702,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -710,7 +712,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -720,7 +722,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -730,7 +732,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -740,7 +742,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -750,7 +752,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -760,7 +762,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -770,7 +772,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -780,7 +782,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -790,7 +792,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -800,7 +802,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -810,7 +812,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -820,7 +822,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>

</xml_diff>